<commit_message>
Updates to the Bug Metrics and Testcases
Co-Authored-By: simshengqin <simshengqin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB14527-BE18-4237-8F20-0A90FC3D80AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09C966E-B921-427A-A10B-32AC0F53301C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Bug Metrics" sheetId="4" r:id="rId2"/>
-    <sheet name="Bug Metric Guide" sheetId="2" r:id="rId3"/>
-    <sheet name="Bug Log Guide" sheetId="3" r:id="rId4"/>
+    <sheet name="Bug Log" sheetId="5" r:id="rId3"/>
+    <sheet name="Bug Metric Guide" sheetId="2" r:id="rId4"/>
+    <sheet name="Bug Log Guide" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="83">
   <si>
     <t>Bug Log</t>
   </si>
@@ -260,6 +261,27 @@
   <si>
     <t xml:space="preserve">Course.csv - Row 4 - Exam Date Column (Blank Exam Date) - Date with space will cause PHP error as validation is unable to compare with data course the system to generator error </t>
   </si>
+  <si>
+    <t xml:space="preserve">Course.csv - Row 5 - Exam Date Column (Date with extra numbers) - Date with extra numbers will cause PHP error as validation is unable to compare with data course the system to generator error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course.csv - Row 15 - Title Column (Delete title) - Date could pass through, when field should not allow empty variables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course.csv - Row 16 - Description Column (Delete description) - deleted description will cause PHP error as validation is unable to compare with data course the system to generator error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course.csv - Row 18 - Course Column (Delete course) - Date could pass through, when field should not allow empty variables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course.csv - Row 22 - School Column (Delete School) - Date could pass through, when field should not allow empty variables </t>
+  </si>
+  <si>
+    <t>Sheng Qin &amp; Vittorio</t>
+  </si>
+  <si>
+    <t>Brednon &amp; DaEun</t>
+  </si>
 </sst>
 </file>
 
@@ -411,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -501,6 +523,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -520,11 +545,251 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="50">
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -963,7 +1228,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1039,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB1AF14-9795-4A94-9B98-2B7CB2042024}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1059,16 +1324,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -1097,48 +1362,48 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="35">
+      <c r="A3" s="36">
         <v>1</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="36">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="35">
+      <c r="F3" s="36">
         <v>1</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="34" t="s">
+      <c r="G3" s="38"/>
+      <c r="H3" s="35" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="34"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="34"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28">
@@ -1229,6 +1494,144 @@
         <v>1</v>
       </c>
       <c r="H9" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="33">
+        <v>6</v>
+      </c>
+      <c r="B10" s="33">
+        <v>1</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="33">
+        <v>1</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="33">
+        <v>7</v>
+      </c>
+      <c r="B11" s="33">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="33">
+        <v>8</v>
+      </c>
+      <c r="B12" s="33">
+        <v>1</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="33">
+        <v>1</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="33">
+        <v>9</v>
+      </c>
+      <c r="B13" s="33">
+        <v>1</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="33">
+        <v>10</v>
+      </c>
+      <c r="B14" s="33">
+        <v>1</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="33">
+        <v>1</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="33">
+        <v>11</v>
+      </c>
+      <c r="B15" s="33">
+        <v>1</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="33">
+        <v>1</v>
+      </c>
+      <c r="H15" s="31" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1245,7 +1648,7 @@
     <mergeCell ref="A3:A5"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H2">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="49" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1255,6 +1658,500 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BA6A9A-5430-4DBB-9166-BAAA04E5944D}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" customWidth="1"/>
+    <col min="4" max="4" width="94.21875" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <f>'Bug Metric Guide'!$A3</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="str">
+        <f>'Bug Metric Guide'!$C3</f>
+        <v>Login (User)</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="12">
+        <v>43738</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <f>'Bug Metric Guide'!$A4</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="12">
+        <v>43739</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="43">
+        <v>3</v>
+      </c>
+      <c r="B5" s="43">
+        <v>1</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="43">
+        <v>4</v>
+      </c>
+      <c r="B6" s="43">
+        <v>1</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="43">
+        <v>5</v>
+      </c>
+      <c r="B7" s="43">
+        <v>1</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="43">
+        <v>6</v>
+      </c>
+      <c r="B8" s="43">
+        <v>1</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <v>7</v>
+      </c>
+      <c r="B9" s="43">
+        <v>1</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
+        <v>8</v>
+      </c>
+      <c r="B10" s="43">
+        <v>1</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
+        <v>9</v>
+      </c>
+      <c r="B11" s="43">
+        <v>1</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>10</v>
+      </c>
+      <c r="B12" s="43">
+        <v>1</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <v>11</v>
+      </c>
+      <c r="B13" s="43">
+        <v>1</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="12">
+        <v>43739</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="containsBlanks" dxfId="30" priority="33">
+      <formula>LEN(TRIM(E3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="containsBlanks" dxfId="27" priority="30">
+      <formula>LEN(TRIM(E4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsBlanks" dxfId="24" priority="27">
+      <formula>LEN(TRIM(E5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="containsBlanks" dxfId="21" priority="24">
+      <formula>LEN(TRIM(E6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsBlanks" dxfId="18" priority="21">
+      <formula>LEN(TRIM(E7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsBlanks" dxfId="15" priority="18">
+      <formula>LEN(TRIM(E8))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsBlanks" dxfId="12" priority="15">
+      <formula>LEN(TRIM(E9))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="containsBlanks" dxfId="9" priority="12">
+      <formula>LEN(TRIM(E10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsBlanks" dxfId="6" priority="9">
+      <formula>LEN(TRIM(E11))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
+      <formula>LEN(TRIM(E12))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Unresolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsBlanks" dxfId="0" priority="3">
+      <formula>LEN(TRIM(E13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="E3:E13" xr:uid="{B948584E-BF58-4B44-BB28-99D97FB97827}">
+      <formula1>"Unresolved,Resolved"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1279,16 +2176,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -1336,7 +2233,7 @@
         <f t="shared" ref="F3:F200" si="0">IF($E3="Critical", 10, IF($E3="High",5, IF($E3="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="36">
         <f>SUM($F3:$F8)</f>
         <v>27</v>
       </c>
@@ -1365,7 +2262,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G4" s="35"/>
+      <c r="G4" s="36"/>
       <c r="H4" s="25"/>
     </row>
     <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1388,7 +2285,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="35"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1411,7 +2308,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G6" s="35"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1434,7 +2331,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="36"/>
       <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -1457,7 +2354,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G8" s="35"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.25">
@@ -1480,7 +2377,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="36">
         <f>SUM(F9:F15)</f>
         <v>20</v>
       </c>
@@ -1509,7 +2406,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10" s="35"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1532,7 +2429,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="35"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1555,7 +2452,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G12" s="35"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1578,7 +2475,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="35"/>
+      <c r="G13" s="36"/>
       <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1601,7 +2498,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G14" s="35"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1624,7 +2521,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G15" s="35"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.25">
@@ -1647,7 +2544,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G16" s="36">
         <f>SUM(F16:F19)</f>
         <v>20</v>
       </c>
@@ -1676,7 +2573,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G17" s="35"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1699,7 +2596,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G18" s="35"/>
+      <c r="G18" s="36"/>
       <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1722,7 +2619,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="35"/>
+      <c r="G19" s="36"/>
       <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.25">
@@ -1745,7 +2642,7 @@
         <f>IF($E20="Critical", 10, IF($E20="High",5, IF($E20="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G20" s="35">
+      <c r="G20" s="36">
         <f>SUM(F20:F23)</f>
         <v>12</v>
       </c>
@@ -1773,7 +2670,7 @@
       <c r="F21" s="21">
         <v>5</v>
       </c>
-      <c r="G21" s="35"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1796,7 +2693,7 @@
         <f>IF($E22="Critical", 10, IF($E22="High",5, IF($E22="Low",1,"")))</f>
         <v>1</v>
       </c>
-      <c r="G22" s="35"/>
+      <c r="G22" s="36"/>
       <c r="H22" s="25"/>
     </row>
     <row r="23" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -1819,7 +2716,7 @@
         <f>IF($E23="Critical", 10, IF($E23="High",5, IF($E23="Low",1,"")))</f>
         <v>5</v>
       </c>
-      <c r="G23" s="35"/>
+      <c r="G23" s="36"/>
       <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
@@ -6949,7 +7846,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Stop current Development">
+    <cfRule type="containsText" dxfId="48" priority="1" operator="containsText" text="Stop current Development">
       <formula>NOT(ISERROR(SEARCH("Stop current Development",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6962,7 +7859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -6970,7 +7867,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6987,16 +7884,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -17400,77 +18297,77 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="13" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="14" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E11 E13:E20">
-    <cfRule type="containsBlanks" dxfId="12" priority="15">
+    <cfRule type="containsBlanks" dxfId="45" priority="15">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="containsBlanks" dxfId="9" priority="12">
+    <cfRule type="containsBlanks" dxfId="42" priority="12">
       <formula>LEN(TRIM(E12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="8" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="containsBlanks" dxfId="6" priority="9">
+    <cfRule type="containsBlanks" dxfId="39" priority="9">
       <formula>LEN(TRIM(E21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="containsBlanks" dxfId="3" priority="6">
+    <cfRule type="containsBlanks" dxfId="36" priority="6">
       <formula>LEN(TRIM(E22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>"Unresolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+    <cfRule type="containsBlanks" dxfId="33" priority="3">
       <formula>LEN(TRIM(E23))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated the Bug logs with recent finds from the UAT
Co-Authored-By: simshengqin <simshengqin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87D611D-54B4-4EAF-8D56-10C753DCF7E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-6465" yWindow="3000" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -17,19 +18,11 @@
     <sheet name="Bug Log" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="62">
   <si>
     <t>Bug Log</t>
   </si>
@@ -218,11 +211,20 @@
   <si>
     <t xml:space="preserve">Add bids instead of update bids when userid and current course exists, causing a exam timetable clash. Should be bid update instead. </t>
   </si>
+  <si>
+    <t>Window Closing</t>
+  </si>
+  <si>
+    <t>When window 2 is closed, there is no prompt to show the current status of the page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When window 2 is closed, there is no prompt to show the current status of the page. This problem is only found in the AWS deployment </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -427,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -491,6 +493,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -525,23 +545,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,20 +872,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="84.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="84.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -888,7 +893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -896,7 +901,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -904,7 +909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -912,11 +917,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -924,7 +929,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -932,7 +937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -946,39 +951,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="84.21875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="84.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="11" customWidth="1"/>
     <col min="6" max="6" width="10" style="11" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="66.109375" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="11"/>
+    <col min="7" max="7" width="15.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="66.140625" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1004,51 +1009,51 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27">
-        <v>1</v>
-      </c>
-      <c r="B3" s="27">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27" t="s">
+    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
+        <v>1</v>
+      </c>
+      <c r="B3" s="33">
+        <v>1</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="27">
-        <v>1</v>
-      </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="24" t="s">
+      <c r="F3" s="33">
+        <v>1</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="25"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="26"/>
-    </row>
-    <row r="6" spans="1:8" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="1:8" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1072,7 +1077,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1096,7 +1101,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>4</v>
       </c>
@@ -1120,7 +1125,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -1144,7 +1149,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>6</v>
       </c>
@@ -1168,7 +1173,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>7</v>
       </c>
@@ -1192,7 +1197,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>8</v>
       </c>
@@ -1216,7 +1221,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>9</v>
       </c>
@@ -1240,7 +1245,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>10</v>
       </c>
@@ -1264,7 +1269,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>11</v>
       </c>
@@ -1288,7 +1293,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>12</v>
       </c>
@@ -1312,17 +1317,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1332,7 +1332,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -1342,7 +1342,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1352,7 +1352,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1362,7 +1362,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -1372,7 +1372,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -1405,38 +1405,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" customWidth="1"/>
-    <col min="4" max="4" width="94.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="94.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>5</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -1766,154 +1766,195 @@
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35">
+    <row r="15" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
         <v>13</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="24">
         <v>3</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="25" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="26">
         <v>43769</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35">
+    <row r="16" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
         <v>14</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="24">
         <v>3</v>
       </c>
-      <c r="C16" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="37" t="s">
+      <c r="C16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>54</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="26">
         <v>43769</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="26">
         <v>43771</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
         <v>15</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="24">
         <v>3</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="25" t="s">
         <v>56</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="38">
+      <c r="F17" s="26">
         <v>43769</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="26">
         <v>43771</v>
       </c>
-      <c r="H17" s="40" t="s">
+      <c r="H17" s="28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35">
+    <row r="18" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
         <v>16</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="24">
         <v>3</v>
       </c>
-      <c r="C18" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="37" t="s">
+      <c r="C18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="26">
         <v>43769</v>
       </c>
-      <c r="G18" s="39"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41">
+        <v>17</v>
+      </c>
+      <c r="B19" s="41">
+        <v>3</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="26">
+        <v>43769</v>
+      </c>
+      <c r="G19" s="26">
+        <v>43771</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
+        <v>18</v>
+      </c>
+      <c r="B20" s="24">
+        <v>3</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="26">
+        <v>43769</v>
+      </c>
+      <c r="G20" s="27"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
bug fix for duplicate student data
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="61">
   <si>
     <t>Bug Log</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t xml:space="preserve">Add bids instead of update bids when userid and current course exists, causing a exam timetable clash. Should be bid update instead. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON - Bootstrap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error field message not sorted </t>
   </si>
 </sst>
 </file>
@@ -491,6 +497,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -525,24 +549,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,7 +955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -967,16 +973,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="A1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -1005,48 +1011,48 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27">
-        <v>1</v>
-      </c>
-      <c r="B3" s="27">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27" t="s">
+      <c r="A3" s="33">
+        <v>1</v>
+      </c>
+      <c r="B3" s="33">
+        <v>1</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="27">
-        <v>1</v>
-      </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="24" t="s">
+      <c r="F3" s="33">
+        <v>1</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="30" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="25"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="26"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:8" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
@@ -1408,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1425,16 +1431,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1767,153 +1773,175 @@
       <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35">
+      <c r="A15" s="23">
         <v>13</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="24">
         <v>3</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="25" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="26">
         <v>43769</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35">
+      <c r="A16" s="23">
         <v>14</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="24">
         <v>3</v>
       </c>
-      <c r="C16" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="37" t="s">
+      <c r="C16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>54</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="26">
         <v>43769</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="26">
         <v>43771</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35">
+      <c r="A17" s="23">
         <v>15</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="24">
         <v>3</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="25" t="s">
         <v>56</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="38">
+      <c r="F17" s="26">
         <v>43769</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="26">
         <v>43771</v>
       </c>
-      <c r="H17" s="40" t="s">
+      <c r="H17" s="28" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35">
+      <c r="A18" s="23">
         <v>16</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="24">
         <v>3</v>
       </c>
-      <c r="C18" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="37" t="s">
+      <c r="C18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="26">
+        <v>43769</v>
+      </c>
+      <c r="G18" s="26">
+        <v>43771</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23">
+        <v>17</v>
+      </c>
+      <c r="B19" s="24">
+        <v>3</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F19" s="26">
         <v>43769</v>
       </c>
-      <c r="G18" s="39"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added validation for add bids: Cannot bid for the same course in a single bid. Added new bugs to the BM
Co-Authored-By: simshengqin <simshengqin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0D7D50-37F3-4937-BA05-4CD3B856FC23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACD1D60-3612-4DC3-9DDD-1A1613F8EC20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1950" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="67">
   <si>
     <t>Bug Log</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>No validation if the vacancy is already at 0 - bid goes through even though there is no vacancy</t>
+  </si>
+  <si>
+    <t>No validation if you bid for two sections of the same course at the same time</t>
+  </si>
+  <si>
+    <t>No validation if you bid for two sections of the same course in separate bids</t>
   </si>
 </sst>
 </file>
@@ -1419,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1974,13 +1980,47 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F24" s="27"/>
+    <row r="23" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="24">
+        <v>3</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="26">
+        <v>43778</v>
+      </c>
+      <c r="G23" s="26">
+        <v>43778</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="26">
+        <v>43778</v>
+      </c>
       <c r="G24" s="27"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F25" s="27"/>

</xml_diff>

<commit_message>
update bm on bug fix
Co-Authored-By: victorweilong <victorweilong@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACD1D60-3612-4DC3-9DDD-1A1613F8EC20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
   <si>
     <t>Bug Log</t>
   </si>
@@ -218,9 +217,6 @@
     <t xml:space="preserve">Error field message not sorted </t>
   </si>
   <si>
-    <t xml:space="preserve">Add bid </t>
-  </si>
-  <si>
     <t>There is an error caused by non-standardized variable names</t>
   </si>
   <si>
@@ -234,12 +230,15 @@
   </si>
   <si>
     <t>No validation if you bid for two sections of the same course in separate bids</t>
+  </si>
+  <si>
+    <t>Should be able to bid even when vacancy is temporarily 0 during round 2. Shouldn't allow bids if round 1 ends, and vacancy is 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -884,20 +883,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="84.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="84.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -905,7 +904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -913,7 +912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -921,7 +920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -929,11 +928,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -941,7 +940,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -949,7 +948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -963,27 +962,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="84.28515625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="84.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="11" customWidth="1"/>
     <col min="6" max="6" width="10" style="11" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="66.140625" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="11"/>
+    <col min="7" max="7" width="15.6640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="66.109375" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
@@ -995,7 +994,7 @@
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
     </row>
-    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33">
         <v>1</v>
       </c>
@@ -1045,7 +1044,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -1055,7 +1054,7 @@
       <c r="G4" s="37"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
@@ -1065,7 +1064,7 @@
       <c r="G5" s="38"/>
       <c r="H5" s="32"/>
     </row>
-    <row r="6" spans="1:8" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1089,7 +1088,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>4</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>6</v>
       </c>
@@ -1185,7 +1184,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>7</v>
       </c>
@@ -1209,7 +1208,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>8</v>
       </c>
@@ -1233,7 +1232,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>9</v>
       </c>
@@ -1257,7 +1256,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>10</v>
       </c>
@@ -1281,7 +1280,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="22">
         <v>11</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20">
         <v>12</v>
       </c>
@@ -1329,7 +1328,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -1339,7 +1338,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1349,7 +1348,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -1359,7 +1358,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1369,7 +1368,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1379,7 +1378,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -1389,7 +1388,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -1422,26 +1421,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="94.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="94.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1452,7 @@
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1479,7 +1478,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -1527,7 +1526,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -1553,7 +1552,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>5</v>
       </c>
@@ -1605,7 +1604,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -1683,7 +1682,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1709,7 +1708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -1735,7 +1734,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -1761,7 +1760,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -1783,7 +1782,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>13</v>
       </c>
@@ -1803,7 +1802,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
         <v>14</v>
       </c>
@@ -1829,7 +1828,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>15</v>
       </c>
@@ -1855,7 +1854,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>16</v>
       </c>
@@ -1881,7 +1880,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>17</v>
       </c>
@@ -1902,7 +1901,7 @@
       </c>
       <c r="G19" s="27"/>
     </row>
-    <row r="20" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>18</v>
       </c>
@@ -1910,10 +1909,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>61</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>62</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>38</v>
@@ -1928,7 +1927,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>19</v>
       </c>
@@ -1936,10 +1935,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>38</v>
@@ -1954,7 +1953,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>20</v>
       </c>
@@ -1962,10 +1961,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>38</v>
@@ -1980,7 +1979,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <v>21</v>
       </c>
@@ -1988,10 +1987,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>38</v>
@@ -2006,12 +2005,18 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23">
+        <v>22</v>
+      </c>
+      <c r="B24" s="24">
+        <v>3</v>
+      </c>
       <c r="C24" s="23" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>25</v>
@@ -2022,35 +2027,57 @@
       <c r="G24" s="27"/>
       <c r="H24" s="28"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23">
+        <v>23</v>
+      </c>
+      <c r="B25" s="24">
+        <v>3</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="26">
+        <v>43778</v>
+      </c>
+      <c r="G25" s="26">
+        <v>43778</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
     </row>

</xml_diff>

<commit_message>
Updated BM for number 24
Co-Authored-By: simshengqin <simshengqin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5C97B1-B2DD-416B-BDC4-A4B872D159BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="30360" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="67">
   <si>
     <t>Bug Log</t>
   </si>
@@ -238,7 +239,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -883,20 +884,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="84.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="84.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -904,7 +905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -912,7 +913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -920,7 +921,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -928,11 +929,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -940,7 +941,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -948,7 +949,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -962,27 +963,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="84.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="84.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="11" customWidth="1"/>
     <col min="6" max="6" width="10" style="11" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="66.109375" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="11"/>
+    <col min="7" max="7" width="15.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="66.140625" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
@@ -994,7 +995,7 @@
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
     </row>
-    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33">
         <v>1</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -1054,7 +1055,7 @@
       <c r="G4" s="37"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
@@ -1064,7 +1065,7 @@
       <c r="G5" s="38"/>
       <c r="H5" s="32"/>
     </row>
-    <row r="6" spans="1:8" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="49.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1088,7 +1089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>4</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>6</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>7</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>8</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>9</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>10</v>
       </c>
@@ -1280,7 +1281,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>11</v>
       </c>
@@ -1304,7 +1305,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>12</v>
       </c>
@@ -1328,7 +1329,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -1338,7 +1339,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1348,7 +1349,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -1358,7 +1359,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1368,7 +1369,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1378,7 +1379,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -1388,7 +1389,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
@@ -1421,26 +1422,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="94.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="94.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1452,7 +1453,7 @@
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>3</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>5</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -1682,7 +1683,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1708,7 +1709,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -1760,7 +1761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -1782,7 +1783,7 @@
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
         <v>13</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>14</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
         <v>15</v>
       </c>
@@ -1854,7 +1855,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>16</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23">
         <v>17</v>
       </c>
@@ -1901,7 +1902,7 @@
       </c>
       <c r="G19" s="27"/>
     </row>
-    <row r="20" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>18</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>19</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>20</v>
       </c>
@@ -1979,7 +1980,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>21</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <v>22</v>
       </c>
@@ -2018,16 +2019,20 @@
       <c r="D24" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>25</v>
+      <c r="E24" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="F24" s="26">
         <v>43778</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
-    </row>
-    <row r="25" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="26">
+        <v>43780</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>23</v>
       </c>
@@ -2053,31 +2058,31 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F32" s="27"/>
       <c r="G32" s="27"/>
     </row>

</xml_diff>

<commit_message>
Found and fixed bug #25. Also made aesthetic changes to drop section
Co-Authored-By: simshengqin <simshengqin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D53BA99-F435-416F-A84A-DA7644BCDE15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C361B60-A08A-48C8-AB3F-CF92AD504631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="71">
   <si>
     <t>Bug Log</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>You can drop a bid once the window is closed. You should only be able to drop bids during active rounds</t>
+  </si>
+  <si>
+    <t>Drop Section</t>
+  </si>
+  <si>
+    <t>You can drop a section once the window is closed. You should only be able to drop sections during active rounds</t>
   </si>
 </sst>
 </file>
@@ -1431,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2090,9 +2096,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
+    <row r="27" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>25</v>
+      </c>
+      <c r="B27" s="24">
+        <v>3</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="26">
+        <v>43780</v>
+      </c>
+      <c r="G27" s="26">
+        <v>43780</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F28" s="27"/>

</xml_diff>

<commit_message>
Fixed bug :Does not show success message or how many lines have been processed. Also updated BM under 26
Co-Authored-By: chadaeun04 <daeun.cha.2018@sis.smu.edu.sg>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C361B60-A08A-48C8-AB3F-CF92AD504631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EF0CFA-686C-44D3-9CDB-C42E2D5CC966}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
   <si>
     <t>Bug Log</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>You can drop a section once the window is closed. You should only be able to drop sections during active rounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boostrap </t>
+  </si>
+  <si>
+    <t>Does not show success message or how many lines have been processed</t>
+  </si>
+  <si>
+    <t>14/11/2019</t>
+  </si>
+  <si>
+    <t>Matthew &amp; DaEun</t>
   </si>
 </sst>
 </file>
@@ -1438,7 +1450,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2122,9 +2134,31 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23">
+        <v>26</v>
+      </c>
+      <c r="B28" s="24">
+        <v>3</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F29" s="27"/>

</xml_diff>

<commit_message>
Fixed bug: Non-consistent bid amounts when clicking on landing page and add bid page. Updated on BM under 27
Co-Authored-By: chadaeun04 <daeun.cha.2018@sis.smu.edu.sg>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EF0CFA-686C-44D3-9CDB-C42E2D5CC966}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5A52F4-FFBE-45D1-B767-10F592534334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15405" yWindow="3375" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
   <si>
     <t>Bug Log</t>
   </si>
@@ -248,9 +248,6 @@
     <t>You can drop a section once the window is closed. You should only be able to drop sections during active rounds</t>
   </si>
   <si>
-    <t xml:space="preserve">Boostrap </t>
-  </si>
-  <si>
     <t>Does not show success message or how many lines have been processed</t>
   </si>
   <si>
@@ -258,6 +255,12 @@
   </si>
   <si>
     <t>Matthew &amp; DaEun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-consistent bid amounts when clicking on landing page and add bid page </t>
   </si>
 </sst>
 </file>
@@ -1449,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2142,27 +2145,49 @@
         <v>3</v>
       </c>
       <c r="C28" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>38</v>
       </c>
       <c r="F28" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="G28" s="26" t="s">
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
+        <v>27</v>
+      </c>
+      <c r="B29" s="27">
+        <v>3</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F30" s="27"/>

</xml_diff>

<commit_message>
Fixed bugs: Not being able to show status result of bids after round 1. Updated BM under 27
Co-Authored-By: chadaeun04 <daeun.cha.2018@sis.smu.edu.sg>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t6\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D102D5-D591-4475-8152-405D51FCF81E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF9561A-754C-4188-980D-9C8697C78B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
   <si>
     <t>Bug Log</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>Sheng Qin &amp; Brendon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landing page </t>
+  </si>
+  <si>
+    <t>Not being able to show status result of bids after round 1</t>
   </si>
 </sst>
 </file>
@@ -891,13 +897,13 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="84.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="84.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -905,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -913,7 +919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -921,7 +927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -929,11 +935,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -941,7 +947,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -949,7 +955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -970,20 +976,20 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="84.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="84.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="11" customWidth="1"/>
     <col min="6" max="6" width="10" style="11" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="66.109375" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="11"/>
+    <col min="7" max="7" width="15.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="66.140625" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
@@ -995,7 +1001,7 @@
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
     </row>
-    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32">
         <v>1</v>
       </c>
@@ -1045,7 +1051,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
@@ -1055,7 +1061,7 @@
       <c r="G4" s="36"/>
       <c r="H4" s="30"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -1065,7 +1071,7 @@
       <c r="G5" s="37"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1113,7 +1119,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>4</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>6</v>
       </c>
@@ -1185,7 +1191,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>7</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>8</v>
       </c>
@@ -1233,7 +1239,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>9</v>
       </c>
@@ -1257,7 +1263,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <v>10</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>11</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -1315,7 +1321,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1325,7 +1331,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -1335,7 +1341,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -1345,7 +1351,7 @@
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -1355,7 +1361,7 @@
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -1365,7 +1371,7 @@
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -1401,23 +1407,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="94.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="94.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -1429,7 +1435,7 @@
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -1507,7 +1513,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -1559,7 +1565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -1585,7 +1591,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -1611,7 +1617,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>8</v>
       </c>
@@ -1663,7 +1669,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1689,7 +1695,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>10</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -1741,7 +1747,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -1767,7 +1773,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>13</v>
       </c>
@@ -1793,7 +1799,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>14</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>15</v>
       </c>
@@ -1845,7 +1851,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>16</v>
       </c>
@@ -1866,7 +1872,7 @@
       </c>
       <c r="G18" s="26"/>
     </row>
-    <row r="19" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>17</v>
       </c>
@@ -1892,7 +1898,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>18</v>
       </c>
@@ -1918,7 +1924,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -1944,7 +1950,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>20</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>21</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>22</v>
       </c>
@@ -2022,7 +2028,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>23</v>
       </c>
@@ -2048,7 +2054,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>24</v>
       </c>
@@ -2074,12 +2080,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>25</v>
       </c>
       <c r="B27" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>71</v>
@@ -2100,12 +2106,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>26</v>
       </c>
       <c r="B28" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>71</v>
@@ -2126,15 +2132,37 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
+        <v>27</v>
+      </c>
+      <c r="B29" s="23">
+        <v>4</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F30" s="26"/>
       <c r="G30" s="26"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
     </row>

</xml_diff>

<commit_message>
Fixed bug on drop section: Money should be refunded when a section is dropped. Updated under BM 28
Co-Authored-By: chadaeun04 <daeun.cha.2018@sis.smu.edu.sg>
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF9561A-754C-4188-980D-9C8697C78B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB1C4EC-18A0-4B6E-ACAE-FA87699C52E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="77">
   <si>
     <t>Bug Log</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Not being able to show status result of bids after round 1</t>
+  </si>
+  <si>
+    <t>Money should be refunded when a section is dropped</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1411,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2158,9 +2161,31 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23">
+        <v>28</v>
+      </c>
+      <c r="B30" s="23">
+        <v>4</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F31" s="26"/>

</xml_diff>

<commit_message>
Fixed bug #31: Error if no file is imported on the bootstrap . Updated BM as well
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t6\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486C334C-6942-4397-93DE-6DF44EFD5ADB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CDEC9D-608B-493F-85E6-D59DF7A20E30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3375" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="84">
   <si>
     <t>Bug Log</t>
   </si>
@@ -259,6 +259,21 @@
   </si>
   <si>
     <t xml:space="preserve">When vacancy reaches max limit, those that were out-bid would causes all other bids status to fail. </t>
+  </si>
+  <si>
+    <t>Admin Page</t>
+  </si>
+  <si>
+    <t>Exclamation mark appears if no file is imported on the admin page</t>
+  </si>
+  <si>
+    <t>Brendon &amp; Vittorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error if no file is imported on the bootstrap </t>
+  </si>
+  <si>
+    <t>16/11/2019</t>
   </si>
 </sst>
 </file>
@@ -462,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -575,6 +590,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,13 +924,13 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="84.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="84.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -920,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -928,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -936,7 +954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -944,11 +962,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -956,7 +974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -964,7 +982,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -985,20 +1003,20 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="84.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="84.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="11" customWidth="1"/>
     <col min="6" max="6" width="10" style="11" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="66.109375" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="11"/>
+    <col min="7" max="7" width="15.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="66.140625" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
@@ -1010,7 +1028,7 @@
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
     </row>
-    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1036,7 +1054,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32">
         <v>1</v>
       </c>
@@ -1060,7 +1078,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
@@ -1070,7 +1088,7 @@
       <c r="G4" s="36"/>
       <c r="H4" s="30"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -1080,7 +1098,7 @@
       <c r="G5" s="37"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1104,7 +1122,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1128,7 +1146,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>4</v>
       </c>
@@ -1152,7 +1170,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -1176,7 +1194,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>6</v>
       </c>
@@ -1200,7 +1218,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>7</v>
       </c>
@@ -1224,7 +1242,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>8</v>
       </c>
@@ -1248,7 +1266,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>9</v>
       </c>
@@ -1272,7 +1290,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <v>10</v>
       </c>
@@ -1296,7 +1314,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>11</v>
       </c>
@@ -1320,7 +1338,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -1330,7 +1348,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1340,7 +1358,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -1350,7 +1368,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -1360,7 +1378,7 @@
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -1370,7 +1388,7 @@
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -1380,7 +1398,7 @@
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -1414,25 +1432,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="94.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="94.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1462,7 @@
       <c r="G1" s="39"/>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1470,7 +1488,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1496,7 +1514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -1522,7 +1540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -1548,7 +1566,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>4</v>
       </c>
@@ -1574,7 +1592,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -1600,7 +1618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>6</v>
       </c>
@@ -1626,7 +1644,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1652,7 +1670,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>8</v>
       </c>
@@ -1678,7 +1696,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1704,7 +1722,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>10</v>
       </c>
@@ -1730,7 +1748,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>11</v>
       </c>
@@ -1756,7 +1774,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>12</v>
       </c>
@@ -1782,7 +1800,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>13</v>
       </c>
@@ -1808,7 +1826,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>14</v>
       </c>
@@ -1834,7 +1852,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>15</v>
       </c>
@@ -1860,7 +1878,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>16</v>
       </c>
@@ -1881,7 +1899,7 @@
       </c>
       <c r="G18" s="26"/>
     </row>
-    <row r="19" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>17</v>
       </c>
@@ -1907,7 +1925,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>18</v>
       </c>
@@ -1933,7 +1951,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -1959,7 +1977,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>20</v>
       </c>
@@ -1985,7 +2003,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>21</v>
       </c>
@@ -2011,7 +2029,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>22</v>
       </c>
@@ -2037,7 +2055,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>23</v>
       </c>
@@ -2063,7 +2081,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>24</v>
       </c>
@@ -2089,7 +2107,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>25</v>
       </c>
@@ -2115,7 +2133,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>26</v>
       </c>
@@ -2141,7 +2159,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="22">
         <v>27</v>
       </c>
@@ -2167,7 +2185,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>28</v>
       </c>
@@ -2193,7 +2211,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
         <v>29</v>
       </c>
@@ -2206,13 +2224,58 @@
       <c r="D31" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>25</v>
+      <c r="E31" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="F31" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23">
+        <v>30</v>
+      </c>
+      <c r="B32" s="23">
+        <v>4</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22">
+        <v>31</v>
+      </c>
+      <c r="B33" s="23">
+        <v>4</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>